<commit_message>
git commit -m "Add excel for intermediate 1 week 3 assessments"
</commit_message>
<xml_diff>
--- a/Excel skills for business/Excel Skills for Business Intermediate I/Week 2/C2-W2-Assessment-Workbook.xlsx
+++ b/Excel skills for business/Excel Skills for Business Intermediate I/Week 2/C2-W2-Assessment-Workbook.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Excel MOOC\002 Course 2 - Intermediate I\02 Week 2\04 Assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prakhar\Downloads\Practice-projects\Excel skills for business\Excel Skills for Business Intermediate I\Week 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421A3E5-57BF-4475-B555-C09DF06D7940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9168"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
   <definedNames>
     <definedName name="ExcelMajorVersion">'Check Digit'!$I$27</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
   <si>
     <t>Part Description</t>
   </si>
@@ -396,15 +397,21 @@
   </si>
   <si>
     <t>As value</t>
+  </si>
+  <si>
+    <t>POST CODE</t>
+  </si>
+  <si>
+    <t>STATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -537,15 +544,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -555,14 +561,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,11 +576,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
-    <cellStyle name="Comma 2" xfId="5"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
@@ -609,14 +614,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -929,20 +934,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L1:M1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="38.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" customWidth="1"/>
     <col min="5" max="5" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -950,23 +957,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="12">
         <f ca="1">IFERROR(ROUND(J18,0)-(TODAY()-42947),"")</f>
-        <v>-326</v>
-      </c>
-      <c r="I1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="13"/>
+      <c r="J1" s="11">
+        <f ca="1">TODAY()</f>
+        <v>45200</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -990,15 +1000,15 @@
       <c r="H3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>2425</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1010,10 +1020,10 @@
       <c r="D4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" t="s">
         <v>91</v>
       </c>
       <c r="G4" s="2">
@@ -1022,14 +1032,17 @@
       <c r="H4" s="1">
         <v>41</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>42913</v>
       </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="6"/>
+      <c r="J4" s="19">
+        <f ca="1">_xlfn.DAYS($J$1,I4)</f>
+        <v>2287</v>
+      </c>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>2213</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1041,10 +1054,10 @@
       <c r="D5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" t="s">
         <v>92</v>
       </c>
       <c r="G5" s="2">
@@ -1053,14 +1066,17 @@
       <c r="H5" s="1">
         <v>33</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>42936</v>
       </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="6"/>
+      <c r="J5" s="19">
+        <f t="shared" ref="J5:J35" ca="1" si="0">_xlfn.DAYS($J$1,I5)</f>
+        <v>2264</v>
+      </c>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>2381</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1072,10 +1088,10 @@
       <c r="D6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" t="s">
         <v>93</v>
       </c>
       <c r="G6" s="2">
@@ -1084,17 +1100,19 @@
       <c r="H6" s="1">
         <v>23</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>42931</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="11"/>
+      <c r="J6" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2269</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>2097</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1103,10 +1121,10 @@
       <c r="D7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" t="s">
         <v>94</v>
       </c>
       <c r="G7" s="2">
@@ -1115,17 +1133,20 @@
       <c r="H7" s="1">
         <v>32</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>42921</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="6"/>
+      <c r="J7" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2279</v>
+      </c>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>2073</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1137,7 +1158,7 @@
       <c r="E8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" t="s">
         <v>94</v>
       </c>
       <c r="G8" s="2">
@@ -1146,29 +1167,32 @@
       <c r="H8" s="1">
         <v>13</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>42904</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="6"/>
+      <c r="J8" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2296</v>
+      </c>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>2290</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" t="s">
         <v>92</v>
       </c>
       <c r="G9" s="2">
@@ -1177,17 +1201,20 @@
       <c r="H9" s="1">
         <v>6</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="9">
         <v>42946</v>
       </c>
-      <c r="J9" s="5"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2254</v>
+      </c>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>2850</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1199,7 +1226,7 @@
       <c r="E10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" t="s">
         <v>94</v>
       </c>
       <c r="G10" s="2">
@@ -1208,14 +1235,17 @@
       <c r="H10" s="1">
         <v>31</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="9">
         <v>42939</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="6"/>
+      <c r="J10" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2261</v>
+      </c>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>2369</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1230,7 +1260,7 @@
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" t="s">
         <v>95</v>
       </c>
       <c r="G11" s="2">
@@ -1239,14 +1269,17 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="9">
         <v>42938</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
+      <c r="J11" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2262</v>
+      </c>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>2082</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1258,10 +1291,10 @@
       <c r="D12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" t="s">
         <v>96</v>
       </c>
       <c r="G12" s="2">
@@ -1270,14 +1303,17 @@
       <c r="H12" s="1">
         <v>23</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="9">
         <v>42902</v>
       </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
+      <c r="J12" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2298</v>
+      </c>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>2485</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1292,7 +1328,7 @@
       <c r="E13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" t="s">
         <v>94</v>
       </c>
       <c r="G13" s="2">
@@ -1301,17 +1337,20 @@
       <c r="H13" s="1">
         <v>28</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="9">
         <v>42918</v>
       </c>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
+      <c r="J13" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2282</v>
+      </c>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>2900</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1323,7 +1362,7 @@
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="2">
@@ -1332,14 +1371,17 @@
       <c r="H14" s="1">
         <v>38</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="9">
         <v>42923</v>
       </c>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
+      <c r="J14" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2277</v>
+      </c>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>2255</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1354,7 +1396,7 @@
       <c r="E15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" t="s">
         <v>94</v>
       </c>
       <c r="G15" s="2">
@@ -1363,14 +1405,17 @@
       <c r="H15" s="1">
         <v>27</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="9">
         <v>42906</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
+      <c r="J15" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2294</v>
+      </c>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>2568</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1385,7 +1430,7 @@
       <c r="E16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" t="s">
         <v>94</v>
       </c>
       <c r="G16" s="2">
@@ -1394,14 +1439,17 @@
       <c r="H16" s="1">
         <v>15</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="9">
         <v>42927</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
+      <c r="J16" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2273</v>
+      </c>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>2676</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1416,7 +1464,7 @@
       <c r="E17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" t="s">
         <v>94</v>
       </c>
       <c r="G17" s="2">
@@ -1425,17 +1473,20 @@
       <c r="H17" s="1">
         <v>19</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>42924</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
+      <c r="J17" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2276</v>
+      </c>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>2658</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" t="s">
         <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1447,7 +1498,7 @@
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" t="s">
         <v>98</v>
       </c>
       <c r="G18" s="2">
@@ -1456,17 +1507,20 @@
       <c r="H18" s="1">
         <v>39</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="9">
         <v>42930</v>
       </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
+      <c r="J18" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2270</v>
+      </c>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
+      <c r="A19" s="6">
         <v>2350</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" t="s">
         <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1475,10 +1529,10 @@
       <c r="D19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" t="s">
         <v>93</v>
       </c>
       <c r="G19" s="2">
@@ -1487,17 +1541,20 @@
       <c r="H19" s="1">
         <v>5</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="9">
         <v>42907</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
+      <c r="J19" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2293</v>
+      </c>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>2252</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1506,10 +1563,10 @@
       <c r="D20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" t="s">
         <v>99</v>
       </c>
       <c r="G20" s="2">
@@ -1518,17 +1575,20 @@
       <c r="H20" s="1">
         <v>30</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>42936</v>
       </c>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
+      <c r="J20" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2264</v>
+      </c>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>2937</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" t="s">
         <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1540,7 +1600,7 @@
       <c r="E21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" t="s">
         <v>99</v>
       </c>
       <c r="G21" s="2">
@@ -1549,17 +1609,20 @@
       <c r="H21" s="1">
         <v>39</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <v>42932</v>
       </c>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
+      <c r="J21" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2268</v>
+      </c>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>2553</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1571,7 +1634,7 @@
       <c r="E22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" t="s">
         <v>99</v>
       </c>
       <c r="G22" s="2">
@@ -1580,17 +1643,20 @@
       <c r="H22" s="1">
         <v>8</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <v>42932</v>
       </c>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
+      <c r="J22" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2268</v>
+      </c>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>2236</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" t="s">
         <v>80</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1602,7 +1668,7 @@
       <c r="E23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" t="s">
         <v>100</v>
       </c>
       <c r="G23" s="2">
@@ -1611,16 +1677,19 @@
       <c r="H23" s="1">
         <v>19</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="9">
         <v>42908</v>
       </c>
-      <c r="J23" s="5"/>
+      <c r="J23" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2292</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>2785</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
         <v>81</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1632,7 +1701,7 @@
       <c r="E24" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" t="s">
         <v>94</v>
       </c>
       <c r="G24" s="2">
@@ -1641,16 +1710,19 @@
       <c r="H24" s="1">
         <v>59</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="9">
         <v>42917</v>
       </c>
-      <c r="J24" s="5"/>
+      <c r="J24" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2283</v>
+      </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>2872</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" t="s">
         <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1662,7 +1734,7 @@
       <c r="E25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" t="s">
         <v>94</v>
       </c>
       <c r="G25" s="2">
@@ -1671,16 +1743,19 @@
       <c r="H25" s="1">
         <v>3</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="9">
         <v>42926</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="J25" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2274</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>2422</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1692,7 +1767,7 @@
       <c r="E26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" t="s">
         <v>99</v>
       </c>
       <c r="G26" s="2">
@@ -1701,16 +1776,19 @@
       <c r="H26" s="1">
         <v>18</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="9">
         <v>42934</v>
       </c>
-      <c r="J26" s="5"/>
+      <c r="J26" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2266</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>2224</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" t="s">
         <v>84</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1722,7 +1800,7 @@
       <c r="E27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" t="s">
         <v>99</v>
       </c>
       <c r="G27" s="2">
@@ -1731,16 +1809,19 @@
       <c r="H27" s="1">
         <v>47</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="9">
         <v>42916</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="J27" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2284</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>2907</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" t="s">
         <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1752,7 +1833,7 @@
       <c r="E28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="2">
@@ -1761,13 +1842,16 @@
       <c r="H28" s="1">
         <v>46</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="9">
         <v>42920</v>
       </c>
-      <c r="J28" s="5"/>
+      <c r="J28" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2280</v>
+      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>2933</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1782,7 +1866,7 @@
       <c r="E29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" t="s">
         <v>94</v>
       </c>
       <c r="G29" s="2">
@@ -1791,13 +1875,16 @@
       <c r="H29" s="1">
         <v>2</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="9">
         <v>42923</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="J29" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2277</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>2133</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -1812,7 +1899,7 @@
       <c r="E30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" t="s">
         <v>94</v>
       </c>
       <c r="G30" s="2">
@@ -1821,13 +1908,16 @@
       <c r="H30" s="1">
         <v>3</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="9">
         <v>42915</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="J30" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2285</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>2675</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -1842,7 +1932,7 @@
       <c r="E31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" t="s">
         <v>94</v>
       </c>
       <c r="G31" s="2">
@@ -1851,13 +1941,16 @@
       <c r="H31" s="1">
         <v>16</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="9">
         <v>42913</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="J31" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2287</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>2932</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1872,7 +1965,7 @@
       <c r="E32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" t="s">
         <v>94</v>
       </c>
       <c r="G32" s="2">
@@ -1881,13 +1974,16 @@
       <c r="H32" s="1">
         <v>21</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="9">
         <v>42924</v>
       </c>
-      <c r="J32" s="5"/>
+      <c r="J32" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2276</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>2452</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1902,7 +1998,7 @@
       <c r="E33" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" t="s">
         <v>94</v>
       </c>
       <c r="G33" s="2">
@@ -1911,13 +2007,16 @@
       <c r="H33" s="1">
         <v>21</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="9">
         <v>42903</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="J33" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2297</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>2035</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -1932,7 +2031,7 @@
       <c r="E34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" t="s">
         <v>94</v>
       </c>
       <c r="G34" s="2">
@@ -1941,16 +2040,19 @@
       <c r="H34" s="1">
         <v>45</v>
       </c>
-      <c r="I34" s="10">
+      <c r="I34" s="9">
         <v>42918</v>
       </c>
-      <c r="J34" s="5"/>
+      <c r="J34" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2282</v>
+      </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>2288</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" t="s">
         <v>73</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1962,7 +2064,7 @@
       <c r="E35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F35" t="s">
         <v>94</v>
       </c>
       <c r="G35" s="2">
@@ -1971,21 +2073,24 @@
       <c r="H35" s="1">
         <v>8</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="9">
         <v>42934</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="J35" s="19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2266</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="J4:J22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J4:J22">
     <sortCondition ref="J4"/>
   </sortState>
   <conditionalFormatting sqref="J1">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>AND($J$1&lt;&gt;(TODAY()),$J$1&lt;&gt;"")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(ExcelMajorVersion&gt;=15,$J$1=TODAY(),NOT(_xlfn.ISFORMULA($J$1)))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>AND($J$1&lt;&gt;(TODAY()),$J$1&lt;&gt;"")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND(ExcelMajorVersion&gt;=15,_xlfn.ISFORMULA($J$1),$J$1=TODAY())</formula>
@@ -2003,11 +2108,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2017,15 +2124,16 @@
     <col min="4" max="4" width="37.21875" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" customWidth="1"/>
     <col min="6" max="6" width="6.109375" customWidth="1"/>
-    <col min="7" max="8" width="6.88671875" style="15" customWidth="1"/>
+    <col min="7" max="8" width="6.88671875" style="13" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.7" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:11" ht="26.7" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="17" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
@@ -2041,269 +2149,1011 @@
       <c r="E4" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="G5" s="17">
+      <c r="H4" s="18"/>
+      <c r="J4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D4, "-",Inventory!A4)</f>
+        <v>SKU-07-2425</v>
+      </c>
+      <c r="B5" s="15" t="str">
+        <f>UPPER(Inventory!C4)</f>
+        <v>GLASS</v>
+      </c>
+      <c r="C5" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E4,5))</f>
+        <v>dynam</v>
+      </c>
+      <c r="D5" s="16" t="str">
+        <f>LEFT(Inventory!B4,FIND(",",Inventory!B4)-1)</f>
+        <v>Solar Glass (Low Iron Tempered)</v>
+      </c>
+      <c r="E5" s="16" t="str">
+        <f>K5&amp;J5</f>
+        <v>NSW2007</v>
+      </c>
+      <c r="G5" s="14">
         <v>1</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="14">
         <f t="array" aca="1" ref="H5:H9" ca="1">TRANSPOSE('Check Digit'!B23:F23)</f>
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="G6" s="17">
+        <v>1767</v>
+      </c>
+      <c r="J5" t="str">
+        <f>MID(Inventory!F4,FIND(",",Inventory!F4)+2,4)</f>
+        <v>2007</v>
+      </c>
+      <c r="K5" t="str">
+        <f>RIGHT(Inventory!F4,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D5, "-",Inventory!A5)</f>
+        <v>SKU-01-2213</v>
+      </c>
+      <c r="B6" s="15" t="str">
+        <f>UPPER(Inventory!C5)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C6" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E5,5))</f>
+        <v>metal</v>
+      </c>
+      <c r="D6" s="16" t="str">
+        <f>LEFT(Inventory!B5,FIND(",",Inventory!B5)-1)</f>
+        <v>Aluminum 6061-T6 Bare Sheet</v>
+      </c>
+      <c r="E6" s="16" t="str">
+        <f t="shared" ref="E6:E36" si="0">K6&amp;J6</f>
+        <v>VIC3182</v>
+      </c>
+      <c r="G6" s="14">
         <v>2</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="14">
         <f ca="1"/>
-        <v>5852</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="G7" s="17">
+        <v>5827</v>
+      </c>
+      <c r="J6" t="str">
+        <f>MID(Inventory!F5,FIND(",",Inventory!F5)+2,4)</f>
+        <v>3182</v>
+      </c>
+      <c r="K6" t="str">
+        <f>RIGHT(Inventory!F5,3)</f>
+        <v>VIC</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D6, "-",Inventory!A6)</f>
+        <v>SKU-12-2381</v>
+      </c>
+      <c r="B7" s="15" t="str">
+        <f>UPPER(Inventory!C6)</f>
+        <v>POLYCARBONATE</v>
+      </c>
+      <c r="C7" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E6,5))</f>
+        <v>harri</v>
+      </c>
+      <c r="D7" s="16" t="str">
+        <f>LEFT(Inventory!B6,FIND(",",Inventory!B6)-1)</f>
+        <v>LEXAN Polycarbonate Sheet</v>
+      </c>
+      <c r="E7" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2010</v>
+      </c>
+      <c r="G7" s="14">
         <v>3</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="14">
         <f ca="1"/>
-        <v>7491</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="G8" s="17">
+        <v>6275</v>
+      </c>
+      <c r="J7" t="str">
+        <f>MID(Inventory!F6,FIND(",",Inventory!F6)+2,4)</f>
+        <v>2010</v>
+      </c>
+      <c r="K7" t="str">
+        <f>RIGHT(Inventory!F6,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D7, "-",Inventory!A7)</f>
+        <v>SKU-15-2097</v>
+      </c>
+      <c r="B8" s="15" t="str">
+        <f>UPPER(Inventory!C7)</f>
+        <v>RUBBER</v>
+      </c>
+      <c r="C8" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E7,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D8" s="16" t="str">
+        <f>LEFT(Inventory!B7,FIND(",",Inventory!B7)-1)</f>
+        <v>Washer</v>
+      </c>
+      <c r="E8" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="G8" s="14">
         <v>4</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="14">
         <f ca="1"/>
-        <v>5800</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="G9" s="17">
+        <v>3203</v>
+      </c>
+      <c r="J8" t="str">
+        <f>MID(Inventory!F7,FIND(",",Inventory!F7)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K8" t="str">
+        <f>RIGHT(Inventory!F7,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D8, "-",Inventory!A8)</f>
+        <v>SKU-17-2073</v>
+      </c>
+      <c r="B9" s="15" t="str">
+        <f>UPPER(Inventory!C8)</f>
+        <v>SILICON</v>
+      </c>
+      <c r="C9" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E8,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D9" s="16" t="str">
+        <f>LEFT(Inventory!B8,FIND(",",Inventory!B8)-1)</f>
+        <v>Sealant/Caulking</v>
+      </c>
+      <c r="E9" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="G9" s="14">
         <v>5</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="14">
         <f ca="1"/>
-        <v>5247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
+        <v>7022</v>
+      </c>
+      <c r="J9" t="str">
+        <f>MID(Inventory!F8,FIND(",",Inventory!F8)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K9" t="str">
+        <f>RIGHT(Inventory!F8,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D9, "-",Inventory!A9)</f>
+        <v>SKU-01-2290</v>
+      </c>
+      <c r="B10" s="15" t="str">
+        <f>UPPER(Inventory!C9)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C10" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E9,5))</f>
+        <v>metal</v>
+      </c>
+      <c r="D10" s="16" t="str">
+        <f>LEFT(Inventory!B9,FIND(",",Inventory!B9)-1)</f>
+        <v>Aluminum 6061-T6</v>
+      </c>
+      <c r="E10" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>VIC3182</v>
+      </c>
+      <c r="J10" t="str">
+        <f>MID(Inventory!F9,FIND(",",Inventory!F9)+2,4)</f>
+        <v>3182</v>
+      </c>
+      <c r="K10" t="str">
+        <f>RIGHT(Inventory!F9,3)</f>
+        <v>VIC</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D10, "-",Inventory!A10)</f>
+        <v>SKU-11-2850</v>
+      </c>
+      <c r="B11" s="15" t="str">
+        <f>UPPER(Inventory!C10)</f>
+        <v>PLASTIC</v>
+      </c>
+      <c r="C11" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E10,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D11" s="16" t="str">
+        <f>LEFT(Inventory!B10,FIND(",",Inventory!B10)-1)</f>
+        <v>Quick-Disconnect Tube Couplings</v>
+      </c>
+      <c r="E11" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J11" t="str">
+        <f>MID(Inventory!F10,FIND(",",Inventory!F10)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K11" t="str">
+        <f>RIGHT(Inventory!F10,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D11, "-",Inventory!A11)</f>
+        <v>SKU-11-2369</v>
+      </c>
+      <c r="B12" s="15" t="str">
+        <f>UPPER(Inventory!C11)</f>
+        <v>PLASTIC</v>
+      </c>
+      <c r="C12" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E11,5))</f>
+        <v>fresh</v>
+      </c>
+      <c r="D12" s="16" t="str">
+        <f>LEFT(Inventory!B11,FIND(",",Inventory!B11)-1)</f>
+        <v>Mini Adjustable Float Valve</v>
+      </c>
+      <c r="E12" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>VIC3121</v>
+      </c>
+      <c r="J12" t="str">
+        <f>MID(Inventory!F11,FIND(",",Inventory!F11)+2,4)</f>
+        <v>3121</v>
+      </c>
+      <c r="K12" t="str">
+        <f>RIGHT(Inventory!F11,3)</f>
+        <v>VIC</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D12, "-",Inventory!A12)</f>
+        <v>SKU-13-2082</v>
+      </c>
+      <c r="B13" s="15" t="str">
+        <f>UPPER(Inventory!C12)</f>
+        <v>POLYETHYLENE</v>
+      </c>
+      <c r="C13" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E12,5))</f>
+        <v xml:space="preserve">foam </v>
+      </c>
+      <c r="D13" s="16" t="str">
+        <f>LEFT(Inventory!B12,FIND(",",Inventory!B12)-1)</f>
+        <v>Closed Cell Foam</v>
+      </c>
+      <c r="E13" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2018</v>
+      </c>
+      <c r="J13" t="str">
+        <f>MID(Inventory!F12,FIND(",",Inventory!F12)+2,4)</f>
+        <v>2018</v>
+      </c>
+      <c r="K13" t="str">
+        <f>RIGHT(Inventory!F12,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D13, "-",Inventory!A13)</f>
+        <v>SKU-19-2485</v>
+      </c>
+      <c r="B14" s="15" t="str">
+        <f>UPPER(Inventory!C13)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C14" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E13,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D14" s="16" t="str">
+        <f>LEFT(Inventory!B13,FIND(",",Inventory!B13)-1)</f>
+        <v>Draw Latches</v>
+      </c>
+      <c r="E14" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J14" t="str">
+        <f>MID(Inventory!F13,FIND(",",Inventory!F13)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K14" t="str">
+        <f>RIGHT(Inventory!F13,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D14, "-",Inventory!A14)</f>
+        <v>SKU-16-2900</v>
+      </c>
+      <c r="B15" s="15" t="str">
+        <f>UPPER(Inventory!C14)</f>
+        <v>SALT</v>
+      </c>
+      <c r="C15" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E14,5))</f>
+        <v>aquar</v>
+      </c>
+      <c r="D15" s="16" t="str">
+        <f>LEFT(Inventory!B14,FIND(",",Inventory!B14)-1)</f>
+        <v>Tropic Marin Sea Salt</v>
+      </c>
+      <c r="E15" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>VIC3181</v>
+      </c>
+      <c r="J15" t="str">
+        <f>MID(Inventory!F14,FIND(",",Inventory!F14)+2,4)</f>
+        <v>3181</v>
+      </c>
+      <c r="K15" t="str">
+        <f>RIGHT(Inventory!F14,3)</f>
+        <v>VIC</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D15, "-",Inventory!A15)</f>
+        <v>SKU-19-2255</v>
+      </c>
+      <c r="B16" s="15" t="str">
+        <f>UPPER(Inventory!C15)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C16" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E15,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D16" s="16" t="str">
+        <f>LEFT(Inventory!B15,FIND(",",Inventory!B15)-1)</f>
+        <v>Cap Screws</v>
+      </c>
+      <c r="E16" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J16" t="str">
+        <f>MID(Inventory!F15,FIND(",",Inventory!F15)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K16" t="str">
+        <f>RIGHT(Inventory!F15,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D16, "-",Inventory!A16)</f>
+        <v>SKU-19-2568</v>
+      </c>
+      <c r="B17" s="15" t="str">
+        <f>UPPER(Inventory!C16)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C17" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E16,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D17" s="16" t="str">
+        <f>LEFT(Inventory!B16,FIND(",",Inventory!B16)-1)</f>
+        <v>Cap Screws</v>
+      </c>
+      <c r="E17" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J17" t="str">
+        <f>MID(Inventory!F16,FIND(",",Inventory!F16)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K17" t="str">
+        <f>RIGHT(Inventory!F16,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D17, "-",Inventory!A17)</f>
+        <v>SKU-19-2676</v>
+      </c>
+      <c r="B18" s="15" t="str">
+        <f>UPPER(Inventory!C17)</f>
+        <v>STEEL</v>
+      </c>
+      <c r="C18" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E17,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D18" s="16" t="str">
+        <f>LEFT(Inventory!B17,FIND(",",Inventory!B17)-1)</f>
+        <v>Cap Screws</v>
+      </c>
+      <c r="E18" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J18" t="str">
+        <f>MID(Inventory!F17,FIND(",",Inventory!F17)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K18" t="str">
+        <f>RIGHT(Inventory!F17,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D18, "-",Inventory!A18)</f>
+        <v>SKU-15-2658</v>
+      </c>
+      <c r="B19" s="15" t="str">
+        <f>UPPER(Inventory!C18)</f>
+        <v>RUBBER</v>
+      </c>
+      <c r="C19" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E18,5))</f>
+        <v>garlo</v>
+      </c>
+      <c r="D19" s="16" t="str">
+        <f>LEFT(Inventory!B18,FIND(",",Inventory!B18)-1)</f>
+        <v>Red SBR Rubber Sheet (Custom Cut Gasket)</v>
+      </c>
+      <c r="E19" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2135</v>
+      </c>
+      <c r="J19" t="str">
+        <f>MID(Inventory!F18,FIND(",",Inventory!F18)+2,4)</f>
+        <v>2135</v>
+      </c>
+      <c r="K19" t="str">
+        <f>RIGHT(Inventory!F18,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D19, "-",Inventory!A19)</f>
+        <v>SKU-09-2350</v>
+      </c>
+      <c r="B20" s="15" t="str">
+        <f>UPPER(Inventory!C19)</f>
+        <v>PAINT</v>
+      </c>
+      <c r="C20" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E19,5))</f>
+        <v>harri</v>
+      </c>
+      <c r="D20" s="16" t="str">
+        <f>LEFT(Inventory!B19,FIND(",",Inventory!B19)-1)</f>
+        <v>Rust-Oleum</v>
+      </c>
+      <c r="E20" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2010</v>
+      </c>
+      <c r="J20" t="str">
+        <f>MID(Inventory!F19,FIND(",",Inventory!F19)+2,4)</f>
+        <v>2010</v>
+      </c>
+      <c r="K20" t="str">
+        <f>RIGHT(Inventory!F19,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D20, "-",Inventory!A20)</f>
+        <v>SKU-11-2252</v>
+      </c>
+      <c r="B21" s="15" t="str">
+        <f>UPPER(Inventory!C20)</f>
+        <v>PLASTIC</v>
+      </c>
+      <c r="C21" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E20,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D21" s="16" t="str">
+        <f>LEFT(Inventory!B20,FIND(",",Inventory!B20)-1)</f>
+        <v>Containment Unit</v>
+      </c>
+      <c r="E21" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J21" t="str">
+        <f>MID(Inventory!F20,FIND(",",Inventory!F20)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K21" t="str">
+        <f>RIGHT(Inventory!F20,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D21, "-",Inventory!A21)</f>
+        <v>SKU-08-2937</v>
+      </c>
+      <c r="B22" s="15" t="str">
+        <f>UPPER(Inventory!C21)</f>
+        <v>OSB</v>
+      </c>
+      <c r="C22" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E21,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D22" s="16" t="str">
+        <f>LEFT(Inventory!B21,FIND(",",Inventory!B21)-1)</f>
+        <v>Backboard</v>
+      </c>
+      <c r="E22" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J22" t="str">
+        <f>MID(Inventory!F21,FIND(",",Inventory!F21)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K22" t="str">
+        <f>RIGHT(Inventory!F21,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D22, "-",Inventory!A22)</f>
+        <v>SKU-10-2553</v>
+      </c>
+      <c r="B23" s="15" t="str">
+        <f>UPPER(Inventory!C22)</f>
+        <v>PE</v>
+      </c>
+      <c r="C23" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E22,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D23" s="16" t="str">
+        <f>LEFT(Inventory!B22,FIND(",",Inventory!B22)-1)</f>
+        <v>Foam Board Insulation LD</v>
+      </c>
+      <c r="E23" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J23" t="str">
+        <f>MID(Inventory!F22,FIND(",",Inventory!F22)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K23" t="str">
+        <f>RIGHT(Inventory!F22,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D23, "-",Inventory!A23)</f>
+        <v>SKU-02-2236</v>
+      </c>
+      <c r="B24" s="15" t="str">
+        <f>UPPER(Inventory!C23)</f>
+        <v>ACRYLIC</v>
+      </c>
+      <c r="C24" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E23,5))</f>
+        <v>roche</v>
+      </c>
+      <c r="D24" s="16" t="str">
+        <f>LEFT(Inventory!B23,FIND(",",Inventory!B23)-1)</f>
+        <v>Brackets</v>
+      </c>
+      <c r="E24" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2204</v>
+      </c>
+      <c r="J24" t="str">
+        <f>MID(Inventory!F23,FIND(",",Inventory!F23)+2,4)</f>
+        <v>2204</v>
+      </c>
+      <c r="K24" t="str">
+        <f>RIGHT(Inventory!F23,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D24, "-",Inventory!A24)</f>
+        <v>SKU-01-2785</v>
+      </c>
+      <c r="B25" s="15" t="str">
+        <f>UPPER(Inventory!C24)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C25" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E24,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D25" s="16" t="str">
+        <f>LEFT(Inventory!B24,FIND(",",Inventory!B24)-1)</f>
+        <v>Reflective Trough</v>
+      </c>
+      <c r="E25" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J25" t="str">
+        <f>MID(Inventory!F24,FIND(",",Inventory!F24)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K25" t="str">
+        <f>RIGHT(Inventory!F24,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D25, "-",Inventory!A25)</f>
+        <v>SKU-04-2872</v>
+      </c>
+      <c r="B26" s="15" t="str">
+        <f>UPPER(Inventory!C25)</f>
+        <v>COPPER</v>
+      </c>
+      <c r="C26" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E25,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D26" s="16" t="str">
+        <f>LEFT(Inventory!B25,FIND(",",Inventory!B25)-1)</f>
+        <v>Receiver Pipe</v>
+      </c>
+      <c r="E26" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J26" t="str">
+        <f>MID(Inventory!F25,FIND(",",Inventory!F25)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K26" t="str">
+        <f>RIGHT(Inventory!F25,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D26, "-",Inventory!A26)</f>
+        <v>SKU-14-2422</v>
+      </c>
+      <c r="B27" s="15" t="str">
+        <f>UPPER(Inventory!C26)</f>
+        <v>PVC</v>
+      </c>
+      <c r="C27" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E26,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D27" s="16" t="str">
+        <f>LEFT(Inventory!B26,FIND(",",Inventory!B26)-1)</f>
+        <v>PVC Pipe</v>
+      </c>
+      <c r="E27" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J27" t="str">
+        <f>MID(Inventory!F26,FIND(",",Inventory!F26)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K27" t="str">
+        <f>RIGHT(Inventory!F26,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D27, "-",Inventory!A27)</f>
+        <v>SKU-14-2224</v>
+      </c>
+      <c r="B28" s="15" t="str">
+        <f>UPPER(Inventory!C27)</f>
+        <v>PVC</v>
+      </c>
+      <c r="C28" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E27,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D28" s="16" t="str">
+        <f>LEFT(Inventory!B27,FIND(",",Inventory!B27)-1)</f>
+        <v>PVC Fittings</v>
+      </c>
+      <c r="E28" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J28" t="str">
+        <f>MID(Inventory!F27,FIND(",",Inventory!F27)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K28" t="str">
+        <f>RIGHT(Inventory!F27,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D28, "-",Inventory!A28)</f>
+        <v>SKU-10-2907</v>
+      </c>
+      <c r="B29" s="15" t="str">
+        <f>UPPER(Inventory!C28)</f>
+        <v>PE</v>
+      </c>
+      <c r="C29" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E28,5))</f>
+        <v>fisch</v>
+      </c>
+      <c r="D29" s="16" t="str">
+        <f>LEFT(Inventory!B28,FIND(",",Inventory!B28)-1)</f>
+        <v>Pipe Insulation LD</v>
+      </c>
+      <c r="E29" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J29" t="str">
+        <f>MID(Inventory!F28,FIND(",",Inventory!F28)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K29" t="str">
+        <f>RIGHT(Inventory!F28,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D29, "-",Inventory!A29)</f>
+        <v>SKU-18-2933</v>
+      </c>
+      <c r="B30" s="15" t="str">
+        <f>UPPER(Inventory!C29)</f>
+        <v>STAINLESS STEEL</v>
+      </c>
+      <c r="C30" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E29,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D30" s="16" t="str">
+        <f>LEFT(Inventory!B29,FIND(",",Inventory!B29)-1)</f>
+        <v>Housing Case</v>
+      </c>
+      <c r="E30" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J30" t="str">
+        <f>MID(Inventory!F29,FIND(",",Inventory!F29)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K30" t="str">
+        <f>RIGHT(Inventory!F29,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D30, "-",Inventory!A30)</f>
+        <v>SKU-05-2133</v>
+      </c>
+      <c r="B31" s="15" t="str">
+        <f>UPPER(Inventory!C30)</f>
+        <v>FIBERGLASS</v>
+      </c>
+      <c r="C31" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E30,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D31" s="16" t="str">
+        <f>LEFT(Inventory!B30,FIND(",",Inventory!B30)-1)</f>
+        <v>Collector Back Insulation</v>
+      </c>
+      <c r="E31" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J31" t="str">
+        <f>MID(Inventory!F30,FIND(",",Inventory!F30)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K31" t="str">
+        <f>RIGHT(Inventory!F30,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D31, "-",Inventory!A31)</f>
+        <v>SKU-04-2675</v>
+      </c>
+      <c r="B32" s="15" t="str">
+        <f>UPPER(Inventory!C31)</f>
+        <v>COPPER</v>
+      </c>
+      <c r="C32" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E31,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D32" s="16" t="str">
+        <f>LEFT(Inventory!B31,FIND(",",Inventory!B31)-1)</f>
+        <v>Receiver Tube</v>
+      </c>
+      <c r="E32" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J32" t="str">
+        <f>MID(Inventory!F31,FIND(",",Inventory!F31)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K32" t="str">
+        <f>RIGHT(Inventory!F31,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D32, "-",Inventory!A32)</f>
+        <v>SKU-01-2932</v>
+      </c>
+      <c r="B33" s="15" t="str">
+        <f>UPPER(Inventory!C32)</f>
+        <v>ALUMINUM</v>
+      </c>
+      <c r="C33" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E32,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D33" s="16" t="str">
+        <f>LEFT(Inventory!B32,FIND(",",Inventory!B32)-1)</f>
+        <v>Absorber Fins</v>
+      </c>
+      <c r="E33" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J33" t="str">
+        <f>MID(Inventory!F32,FIND(",",Inventory!F32)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K33" t="str">
+        <f>RIGHT(Inventory!F32,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D33, "-",Inventory!A33)</f>
+        <v>SKU-06-2452</v>
+      </c>
+      <c r="B34" s="15" t="str">
+        <f>UPPER(Inventory!C33)</f>
+        <v>FOAM</v>
+      </c>
+      <c r="C34" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E33,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D34" s="16" t="str">
+        <f>LEFT(Inventory!B33,FIND(",",Inventory!B33)-1)</f>
+        <v>Pipe Insulation</v>
+      </c>
+      <c r="E34" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J34" t="str">
+        <f>MID(Inventory!F33,FIND(",",Inventory!F33)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K34" t="str">
+        <f>RIGHT(Inventory!F33,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D34, "-",Inventory!A34)</f>
+        <v>SKU-06-2035</v>
+      </c>
+      <c r="B35" s="15" t="str">
+        <f>UPPER(Inventory!C34)</f>
+        <v>FOAM</v>
+      </c>
+      <c r="C35" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E34,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D35" s="16" t="str">
+        <f>LEFT(Inventory!B34,FIND(",",Inventory!B34)-1)</f>
+        <v>Pipe Insulation</v>
+      </c>
+      <c r="E35" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J35" t="str">
+        <f>MID(Inventory!F34,FIND(",",Inventory!F34)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K35" t="str">
+        <f>RIGHT(Inventory!F34,3)</f>
+        <v>NSW</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="str">
+        <f>_xlfn.CONCAT("SKU-", Inventory!D35, "-",Inventory!A35)</f>
+        <v>SKU-17-2288</v>
+      </c>
+      <c r="B36" s="15" t="str">
+        <f>UPPER(Inventory!C35)</f>
+        <v>SILICON</v>
+      </c>
+      <c r="C36" s="15" t="str">
+        <f>LOWER(LEFT(Inventory!E35,5))</f>
+        <v>pensh</v>
+      </c>
+      <c r="D36" s="16" t="str">
+        <f>LEFT(Inventory!B35,FIND(",",Inventory!B35)-1)</f>
+        <v>Sealant/Caulking</v>
+      </c>
+      <c r="E36" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>NSW2000</v>
+      </c>
+      <c r="J36" t="str">
+        <f>MID(Inventory!F35,FIND(",",Inventory!F35)+2,4)</f>
+        <v>2000</v>
+      </c>
+      <c r="K36" t="str">
+        <f>RIGHT(Inventory!F35,3)</f>
+        <v>NSW</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2315,7 +3165,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I30"/>
   <sheetViews>
@@ -2323,8 +3173,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="12.21875" style="16" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="6" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
@@ -2350,15 +3199,15 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="str">
+      <c r="A5" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D4&amp;"-"&amp;Inventory!A4</f>
         <v>SKU-07-2425</v>
       </c>
-      <c r="B5" s="16" t="str">
+      <c r="B5" t="str">
         <f>UPPER(Inventory!C4)</f>
         <v>GLASS</v>
       </c>
-      <c r="C5" s="16" t="str">
+      <c r="C5" t="str">
         <f>LOWER(LEFT(Inventory!E4,5))</f>
         <v>dynam</v>
       </c>
@@ -2372,15 +3221,15 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="str">
+      <c r="A6" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D5&amp;"-"&amp;Inventory!A5</f>
         <v>SKU-01-2213</v>
       </c>
-      <c r="B6" s="16" t="str">
+      <c r="B6" t="str">
         <f>UPPER(Inventory!C5)</f>
         <v>ALUMINUM</v>
       </c>
-      <c r="C6" s="16" t="str">
+      <c r="C6" t="str">
         <f>LOWER(LEFT(Inventory!E5,5))</f>
         <v>metal</v>
       </c>
@@ -2394,15 +3243,15 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="str">
+      <c r="A7" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D6&amp;"-"&amp;Inventory!A6</f>
         <v>SKU-12-2381</v>
       </c>
-      <c r="B7" s="16" t="str">
+      <c r="B7" t="str">
         <f>UPPER(Inventory!C6)</f>
         <v>POLYCARBONATE</v>
       </c>
-      <c r="C7" s="16" t="str">
+      <c r="C7" t="str">
         <f>LOWER(LEFT(Inventory!E6,5))</f>
         <v>harri</v>
       </c>
@@ -2416,15 +3265,15 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="str">
+      <c r="A8" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D7&amp;"-"&amp;Inventory!A7</f>
         <v>SKU-15-2097</v>
       </c>
-      <c r="B8" s="16" t="str">
+      <c r="B8" t="str">
         <f>UPPER(Inventory!C7)</f>
         <v>RUBBER</v>
       </c>
-      <c r="C8" s="16" t="str">
+      <c r="C8" t="str">
         <f>LOWER(LEFT(Inventory!E7,5))</f>
         <v>pensh</v>
       </c>
@@ -2438,15 +3287,15 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="str">
+      <c r="A9" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D8&amp;"-"&amp;Inventory!A8</f>
         <v>SKU-17-2073</v>
       </c>
-      <c r="B9" s="16" t="str">
+      <c r="B9" t="str">
         <f>UPPER(Inventory!C8)</f>
         <v>SILICON</v>
       </c>
-      <c r="C9" s="16" t="str">
+      <c r="C9" t="str">
         <f>LOWER(LEFT(Inventory!E8,5))</f>
         <v>pensh</v>
       </c>
@@ -2460,15 +3309,15 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="str">
+      <c r="A10" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D9&amp;"-"&amp;Inventory!A9</f>
         <v>SKU-01-2290</v>
       </c>
-      <c r="B10" s="16" t="str">
+      <c r="B10" t="str">
         <f>UPPER(Inventory!C9)</f>
         <v>ALUMINUM</v>
       </c>
-      <c r="C10" s="16" t="str">
+      <c r="C10" t="str">
         <f>LOWER(LEFT(Inventory!E9,5))</f>
         <v>metal</v>
       </c>
@@ -2482,15 +3331,15 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="str">
+      <c r="A11" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D10&amp;"-"&amp;Inventory!A10</f>
         <v>SKU-11-2850</v>
       </c>
-      <c r="B11" s="16" t="str">
+      <c r="B11" t="str">
         <f>UPPER(Inventory!C10)</f>
         <v>PLASTIC</v>
       </c>
-      <c r="C11" s="16" t="str">
+      <c r="C11" t="str">
         <f>LOWER(LEFT(Inventory!E10,5))</f>
         <v>pensh</v>
       </c>
@@ -2504,15 +3353,15 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="str">
+      <c r="A12" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D11&amp;"-"&amp;Inventory!A11</f>
         <v>SKU-11-2369</v>
       </c>
-      <c r="B12" s="16" t="str">
+      <c r="B12" t="str">
         <f>UPPER(Inventory!C11)</f>
         <v>PLASTIC</v>
       </c>
-      <c r="C12" s="16" t="str">
+      <c r="C12" t="str">
         <f>LOWER(LEFT(Inventory!E11,5))</f>
         <v>fresh</v>
       </c>
@@ -2526,15 +3375,15 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="str">
+      <c r="A13" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D12&amp;"-"&amp;Inventory!A12</f>
         <v>SKU-13-2082</v>
       </c>
-      <c r="B13" s="16" t="str">
+      <c r="B13" t="str">
         <f>UPPER(Inventory!C12)</f>
         <v>POLYETHYLENE</v>
       </c>
-      <c r="C13" s="16" t="str">
+      <c r="C13" t="str">
         <f>LOWER(LEFT(Inventory!E12,5))</f>
         <v xml:space="preserve">foam </v>
       </c>
@@ -2548,15 +3397,15 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="str">
+      <c r="A14" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D13&amp;"-"&amp;Inventory!A13</f>
         <v>SKU-19-2485</v>
       </c>
-      <c r="B14" s="16" t="str">
+      <c r="B14" t="str">
         <f>UPPER(Inventory!C13)</f>
         <v>STEEL</v>
       </c>
-      <c r="C14" s="16" t="str">
+      <c r="C14" t="str">
         <f>LOWER(LEFT(Inventory!E13,5))</f>
         <v>pensh</v>
       </c>
@@ -2570,15 +3419,15 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="str">
+      <c r="A15" t="str">
         <f>"SKU"&amp;"-"&amp;Inventory!D14&amp;"-"&amp;Inventory!A14</f>
         <v>SKU-16-2900</v>
       </c>
-      <c r="B15" s="16" t="str">
+      <c r="B15" t="str">
         <f>UPPER(Inventory!C14)</f>
         <v>SALT</v>
       </c>
-      <c r="C15" s="16" t="str">
+      <c r="C15" t="str">
         <f>LOWER(LEFT(Inventory!E14,5))</f>
         <v>aquar</v>
       </c>
@@ -2592,25 +3441,23 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17"/>
-      <c r="B17" s="16" t="s">
+      <c r="B17" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2618,19 +3465,19 @@
       <c r="A18" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18">
         <v>1767</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18">
         <v>5827</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18">
         <v>6275</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18">
         <v>3203</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18">
         <v>7022</v>
       </c>
     </row>
@@ -2638,19 +3485,19 @@
       <c r="A19" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19">
         <v>7385</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19">
         <v>4147</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19">
         <v>2783</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19">
         <v>2790</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19">
         <v>6536</v>
       </c>
     </row>
@@ -2658,19 +3505,19 @@
       <c r="A20" t="s">
         <v>105</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20">
         <v>1299</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20">
         <v>5852</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20">
         <v>7491</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20">
         <v>5800</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20">
         <v>5247</v>
       </c>
     </row>
@@ -2678,24 +3525,23 @@
       <c r="A21" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21">
         <v>3287</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21">
         <v>2614</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21">
         <v>5566</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21">
         <v>6986</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21">
         <v>7560</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
@@ -2703,145 +3549,145 @@
       <c r="A23" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23">
         <f ca="1">IF(AND(B25,EXACT('For Printing'!A8,A8)),B18,IF(B25,B19,IF('For Printing'!A8="",B20,B21)))</f>
-        <v>1299</v>
-      </c>
-      <c r="C23" s="16">
+        <v>1767</v>
+      </c>
+      <c r="C23">
         <f ca="1">IF(AND(C25,EXACT('For Printing'!B8,B8)),C18,IF(C25,C19,IF('For Printing'!B8="",C20,C21)))</f>
-        <v>5852</v>
-      </c>
-      <c r="D23" s="16">
+        <v>5827</v>
+      </c>
+      <c r="D23">
         <f ca="1">IF(AND(D25,EXACT('For Printing'!C8,C8)),D18,IF(D25,D19,IF('For Printing'!C8="",D20,D21)))</f>
-        <v>7491</v>
-      </c>
-      <c r="E23" s="16">
+        <v>6275</v>
+      </c>
+      <c r="E23">
         <f ca="1">IF(AND(E25,EXACT('For Printing'!D8,D8)),E18,IF(E25,E19,IF('For Printing'!D8="",E20,E21)))</f>
-        <v>5800</v>
-      </c>
-      <c r="F23" s="16">
+        <v>3203</v>
+      </c>
+      <c r="F23">
         <f ca="1">IF(AND(F25,EXACT('For Printing'!E8,E8)),F18,IF(F25,F19,IF('For Printing'!E8="",F20,F21)))</f>
-        <v>5247</v>
+        <v>7022</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+      <c r="A25" t="s">
         <v>116</v>
       </c>
-      <c r="B25" s="16" t="b">
+      <c r="B25" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,B28,B27)</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C25" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,C28,C27)</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,D28,D27)</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,E28,E27)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" t="b">
         <f ca="1">IF(ExcelMajorVersion&gt;=15,F28,F27)</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="16" t="str">
+      <c r="I25" t="str">
         <f ca="1">TRIM(CLEAN(INFO("RELEASE")))</f>
         <v>16.0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H26" s="16" t="s">
+      <c r="H26" t="s">
         <v>120</v>
       </c>
-      <c r="I26" s="16" t="str">
+      <c r="I26" t="str">
         <f ca="1">LEFT(I25,FIND(".",I25)-1)</f>
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="16" t="b">
+      <c r="B27" t="b">
         <v>1</v>
       </c>
-      <c r="C27" s="16" t="b">
+      <c r="C27" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="16" t="b">
+      <c r="D27" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="16" t="b">
+      <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="16" t="b">
+      <c r="F27" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" t="s">
         <v>121</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27">
         <f ca="1">VALUE(I26)</f>
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="16" t="b">
+      <c r="B28" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!A8),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="C28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C28" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!B8),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!C8),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!D8),FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
         <f>IFERROR(_xlfn.ISFORMULA('For Printing'!E8),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
+      <c r="A30" t="s">
         <v>114</v>
       </c>
-      <c r="B30" s="16" t="b">
+      <c r="B30" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!A8),CELL("prefix",'For Printing'!A8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!A8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!B8),CELL("prefix",'For Printing'!B8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!B8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!C8),CELL("prefix",'For Printing'!C8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!C8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!D8),CELL("prefix",'For Printing'!D8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!D8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" t="b">
         <f ca="1">IF(OR(ISBLANK('For Printing'!E8),CELL("prefix",'For Printing'!E8)&lt;&gt;""),FALSE,IF(CELL("type",'For Printing'!E8)="l",TRUE,"MAYBE"))</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>